<commit_message>
Added angular authentication project one more time
</commit_message>
<xml_diff>
--- a/python/bni.xlsx
+++ b/python/bni.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,377 +434,266 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>A Chandra Sekhar Om sai prasad plylams Retail &gt; Wood Merchants 9840171190</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Anuvarshini K M Malmur Architects Architecture &amp; Engineering &gt; Architect 9444674365</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Aravind J JOY ENGINEERING AND ENERGY Construction &gt; Solar 9962420007</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Aravindan Sriramulu Profin Solutions Finance &amp; Insurance &gt; Commercial Loans 9841049913</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Austin Anandkumar D&amp;A Events Event &amp; Business Service &gt; Events 9841074842</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Balachandar Srinivasan Shree Baby Caterers Food &amp; Beverage &gt; Caterer 9841549311</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Balasubramaniam T Veecare Properties Real Estate Services &gt; Real Estate Planning Consultant 9841070699</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Chandru Chakrapani Peogic Solutions Employment Activities &gt; Human Resources 9840056921</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Dinesh Kumar N Vel Studios Advertising &amp; Marketing &gt; Photographer 7200141182</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>Dr Sharmila . Inspera Education and Healthcare Pvt Ltd Training &amp; Coaching &gt; Education Services/Tutor 9999983199</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Dr.Bhagyalakshmi V Elysian Handmade Skin &amp; Hair Care Personal Services &gt; Cosmetics/Skin Care 9940494156</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Karthideepan .T Impeccable Infrastructure Solution Construction &gt; Interior Design - Commercial 9042021986</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Khader Shareef Khader Shareef Finance &amp; Insurance &gt; Life and Disability Insurance 98413 36295</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Krishnan Ranganathan CHENNAI CARS Car &amp; Motorcycle &gt; Auto/Car Repair 9840124365</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>Kunal Todi TODI ASSOCIATES Manufacturing &gt; Manufacturing (Other) 9840448144</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
+      <c r="A17" t="inlineStr">
         <is>
           <t>Maheswaran Maheswaran Star Litho Advertising &amp; Marketing &gt; Sign Company 9884881191</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
+      <c r="A18" t="inlineStr">
         <is>
           <t>Malaichamy .K Hybrid Network Solutions Retail &gt; Computer Accessories 9940096377</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
+      <c r="A19" t="inlineStr">
         <is>
           <t>Moorthy D Mootek Technologies Car &amp; Motorcycle &gt; Car &amp; Motorcycle (Other) 04442821520</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
+      <c r="A20" t="inlineStr">
         <is>
           <t>Muthuvel .P Sri Bala Sai Decors Construction &gt; Construction (Other) 7358365778</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
+      <c r="A21" t="inlineStr">
         <is>
           <t>Pinky Rajesh URChoice Corporate Gifting Private Limited Retail &gt; Gifts 9176676699</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
+      <c r="A22" t="inlineStr">
         <is>
           <t>Prabhu .D Construction &gt; HVAC - Heating &amp; Air 044-25564737</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
+      <c r="A23" t="inlineStr">
         <is>
           <t>Priyanka Girdonia E Giraffes Advertising &amp; Marketing &gt; Digital Marketing 9176367409</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
+      <c r="A24" t="inlineStr">
         <is>
           <t>Raaju P PRS Associates Advertising &amp; Marketing &gt; Printer 9841215354</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
+      <c r="A25" t="inlineStr">
         <is>
           <t>RAJA MUNUSAMY INSURANZ HUB Finance &amp; Insurance &gt; General Insurance 9094514168</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
+      <c r="A26" t="inlineStr">
         <is>
           <t>Rajeswari M. RAF Finance &amp; Insurance &gt; Finance &amp; Insurance (Other) +91 9789875872</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
+      <c r="A27" t="inlineStr">
         <is>
           <t>Rajkumar Pandian Raja electricals n hardwares Retail &gt; Construction Products Retail 9840762940</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
+      <c r="A28" t="inlineStr">
         <is>
           <t>Ramarajan D winsome power technologies pvt ltd Construction &gt; Electrician - Commercial 9952695122</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
+      <c r="A29" t="inlineStr">
         <is>
           <t>Ramesh R Digitpro Security &amp; Investigation &gt; Fire Protection 9176644406</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
+      <c r="A30" t="inlineStr">
         <is>
           <t>Rathi Azhaguraj Azhagupattarai Personal Services &gt; Personal Services (Other) 9940140522</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
+      <c r="A31" t="inlineStr">
         <is>
           <t>Saipriya Dharshini Swaaadle Tech Pvt Ltd Retail &gt; Retail (Other) 9884128527</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
+      <c r="A32" t="inlineStr">
         <is>
           <t>Sathiaseelan K S SS CONSTRUCTIONS Construction &gt; Builder/General Contractor 9444521467</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
+      <c r="A33" t="inlineStr">
         <is>
           <t>Shankar Ganesh E SG TECH Construction &gt; HVAC - Heating &amp; Air 8015543555</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
+      <c r="A34" t="inlineStr">
         <is>
           <t>Shibu P K Biocosmo Health Care Health &amp; Wellness &gt; Health &amp; Wellness Services 7200080075</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
+      <c r="A35" t="inlineStr">
         <is>
           <t>Sivaa Rajkumar Scoobys Cafe Food &amp; Beverage &gt; Beverage Service 7358094353</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
+      <c r="A36" t="inlineStr">
         <is>
           <t>Srinivasan .R BrickBus Technologies Private Limited Retail &gt; Building Materials 8754792793</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
+      <c r="A37" t="inlineStr">
         <is>
           <t>Suriya Moorthy G SS FACILITY SERVICES Personal Services &gt; Personal Services (Other) 9884237753</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
+      <c r="A38" t="inlineStr">
         <is>
           <t>Thirumal Rao .M.S Datatech communications Telecommunications &gt; Telecommunications Products/Services 9841053515</t>
         </is>

</xml_diff>